<commit_message>
Hemos hecho algunas mejoras en el script como hacer que los mails solo se gestionen del archivo config.json y no del archivo encargados.xlsx
</commit_message>
<xml_diff>
--- a/data/input/encargados.xlsx
+++ b/data/input/encargados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALMACENAMIENTO\Ivan\viveverde\Trabajos\IA\vivero_pedidos\PROGRAMA_PEDIDOS\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89AEF06-A71B-4B07-8B36-6C5EE89B61DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B55CC9C-1696-4F2E-A191-70C1EFC84957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="-15555" windowWidth="21600" windowHeight="11835" xr2:uid="{32E8CE30-D129-4F75-97B4-F9098B36F8CE}"/>
+    <workbookView xWindow="6105" yWindow="-14295" windowWidth="21600" windowHeight="11835" xr2:uid="{32E8CE30-D129-4F75-97B4-F9098B36F8CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>mail</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve"> seccion/es</t>
   </si>
@@ -47,58 +44,37 @@
     <t>Iris</t>
   </si>
   <si>
-    <t>interior@viveverde.es</t>
-  </si>
-  <si>
     <t>interior</t>
   </si>
   <si>
     <t>María</t>
   </si>
   <si>
-    <t>mascotas@gmail.com</t>
-  </si>
-  <si>
     <t>mascotas_Manufacturado, Mascotas_vivo</t>
   </si>
   <si>
     <t>Pablo</t>
   </si>
   <si>
-    <t>deco.exterior@viveverde.es</t>
-  </si>
-  <si>
     <t>deco_exterior, tierras_aridos</t>
   </si>
   <si>
     <t>Ivan</t>
   </si>
   <si>
-    <t>ivan.delgado@viveverde.es</t>
-  </si>
-  <si>
     <t>Fitos, semillas, utiles_jardin</t>
   </si>
   <si>
     <t>Rocío</t>
   </si>
   <si>
-    <t>decoracion@viveverde.es</t>
-  </si>
-  <si>
     <t>deco_interior</t>
   </si>
   <si>
     <t>Sandra</t>
   </si>
   <si>
-    <t>sandra.delgado@viveverde.es</t>
-  </si>
-  <si>
     <t>Jose</t>
-  </si>
-  <si>
-    <t>exterior@viveverde.es</t>
   </si>
   <si>
     <t>maf, vivero</t>
@@ -111,18 +87,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,23 +141,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,117 +487,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F3FF12-703A-4C24-AB80-1246BB47B558}">
-  <dimension ref="I7:K14"/>
+  <dimension ref="I7:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="9:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="I7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="3" t="s">
+    <row r="7" spans="9:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="3" t="s">
+    </row>
+    <row r="8" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="2" t="s">
+    </row>
+    <row r="9" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="1" t="s">
+    <row r="10" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="1" t="s">
+    </row>
+    <row r="11" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I10" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="2" t="s">
+    </row>
+    <row r="12" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="1" t="s">
+    <row r="13" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{DC442DC0-153B-4F39-A4EE-F5C00B8B1278}"/>
-    <hyperlink ref="J9" r:id="rId2" xr:uid="{626E0972-2578-4746-8BA4-BD6AA8965A24}"/>
-    <hyperlink ref="J10" r:id="rId3" xr:uid="{EE2C5211-00FC-4DF0-BEA1-5CFDCE0CFDEF}"/>
-    <hyperlink ref="J11" r:id="rId4" xr:uid="{94EA3FC5-62C6-4A27-B453-0000ED83E37D}"/>
-    <hyperlink ref="J12" r:id="rId5" xr:uid="{C2CB645F-479B-447C-9F49-98C1858978AE}"/>
-    <hyperlink ref="J13" r:id="rId6" xr:uid="{64D4ED9E-317A-4181-BFF7-4C27AC2AF8AD}"/>
-    <hyperlink ref="J14" r:id="rId7" xr:uid="{4C99B717-D56C-45CE-A4D2-82217DA1E997}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hemos hecho que el mail sea nominativo para cada encargado
</commit_message>
<xml_diff>
--- a/data/input/encargados.xlsx
+++ b/data/input/encargados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALMACENAMIENTO\Ivan\viveverde\Trabajos\IA\vivero_pedidos\PROGRAMA_PEDIDOS\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B55CC9C-1696-4F2E-A191-70C1EFC84957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5B5B70-0788-436F-8B69-6BABC736DF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6105" yWindow="-14295" windowWidth="21600" windowHeight="11835" xr2:uid="{32E8CE30-D129-4F75-97B4-F9098B36F8CE}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="I7:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>